<commit_message>
update to merge gear model
</commit_message>
<xml_diff>
--- a/ArticleCollision.xlsx
+++ b/ArticleCollision.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://correounivalleeduco-my.sharepoint.com/personal/jaime_cuartas_correounivalle_edu_co/Documents/Documentos/Github/TranslationTraceUppaal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9503BB2B-D60E-4584-98D7-3E17ED6DFB2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{9503BB2B-D60E-4584-98D7-3E17ED6DFB2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E531F00A-660B-4AF9-8AA9-2731A45EE889}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{CC4AB360-C031-4987-BA78-0B792974B2C5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CC4AB360-C031-4987-BA78-0B792974B2C5}"/>
   </bookViews>
   <sheets>
     <sheet name="PosBisimilar" sheetId="2" r:id="rId1"/>
@@ -426,51 +426,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5366ABA3-A402-4A32-BDFA-6F382EF64E3E}" name="similarTraces" displayName="similarTraces" ref="A1:D481" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:D481" xr:uid="{5366ABA3-A402-4A32-BDFA-6F382EF64E3E}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="smiTemplateid1.xml"/>
-        <filter val="smiTemplateid4.xml"/>
-        <filter val="tadSyncid0id0.xml"/>
-        <filter val="tadSyncid0id2.xml"/>
-        <filter val="tadSyncid0id3.xml"/>
-        <filter val="tadSyncid0id4.xml"/>
-        <filter val="tadSyncid0id5.xml"/>
-        <filter val="tadSyncid1id2.xml"/>
-        <filter val="tadSyncid1id4.xml"/>
-        <filter val="tadSyncid1id5.xml"/>
-        <filter val="tadSyncid2id0.xml"/>
-        <filter val="tadSyncid2id1.xml"/>
-        <filter val="tadSyncid2id3.xml"/>
-        <filter val="tadSyncid2id4.xml"/>
-        <filter val="tadSyncid3id0.xml"/>
-        <filter val="tadSyncid3id1.xml"/>
-        <filter val="tadSyncid3id2.xml"/>
-        <filter val="tadSyncid3id3.xml"/>
-        <filter val="tadSyncid3id4.xml"/>
-        <filter val="tadSyncid4id1.xml"/>
-        <filter val="tadSyncid4id3.xml"/>
-        <filter val="tadSyncid5id0.xml"/>
-        <filter val="tadSyncid5id1.xml"/>
-        <filter val="tadSyncid5id2.xml"/>
-        <filter val="tmi1.xml"/>
-        <filter val="tmi10.xml"/>
-        <filter val="tmi11.xml"/>
-        <filter val="tmi12.xml"/>
-        <filter val="tmi13.xml"/>
-        <filter val="tmi2.xml"/>
-        <filter val="tmi4.xml"/>
-        <filter val="tmi6.xml"/>
-        <filter val="tmi9.xml"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="1">
-      <filters>
-        <filter val="ccn1.xml"/>
-        <filter val="ccn2.xml"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:D481" xr:uid="{5366ABA3-A402-4A32-BDFA-6F382EF64E3E}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{4A5EE59D-B58D-49A8-9A26-F4FB760BAF37}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{3D862906-4B5B-4FED-BCDD-EF9130A64049}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="4"/>
@@ -485,8 +441,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{978AA107-72F0-44DE-9D9F-FFDA46E16674}" name="similarTraces__4" displayName="similarTraces__4" ref="A1:D341" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:D341" xr:uid="{978AA107-72F0-44DE-9D9F-FFDA46E16674}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{8B9DE20A-58E6-4893-B087-B593A597FC0F}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{86849DC3-9064-4E97-94BF-A3F59AF9277B}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{8B9DE20A-58E6-4893-B087-B593A597FC0F}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{86849DC3-9064-4E97-94BF-A3F59AF9277B}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{0D186F94-E996-4879-9EB7-B95B03758A9D}" uniqueName="3" name="Column3" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{C33BAB95-C3B7-4219-A352-6A4B0FB81187}" uniqueName="4" name="Column4" queryTableFieldId="4"/>
   </tableColumns>
@@ -547,8 +503,8 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{BCE78EDD-51D5-4707-9394-C6CFB87313E1}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{94C4EF0B-A647-4162-9C35-CC25A084A9CC}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{BCE78EDD-51D5-4707-9394-C6CFB87313E1}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{94C4EF0B-A647-4162-9C35-CC25A084A9CC}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{E4125180-8D18-485B-A8A8-FC07FB6F476F}" uniqueName="3" name="Column3" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{67C29ED7-92AD-434A-B099-098894EAE92B}" uniqueName="4" name="Column4" queryTableFieldId="4"/>
   </tableColumns>
@@ -855,8 +811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DB39ED0-650C-4180-875A-F1E2AF2595D5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView topLeftCell="A412" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:A455"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -880,7 +836,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -894,7 +850,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -908,7 +864,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -922,7 +878,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -936,7 +892,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -950,7 +906,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -964,7 +920,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -978,7 +934,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -992,7 +948,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
@@ -1006,7 +962,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
@@ -1020,7 +976,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
@@ -1034,7 +990,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
@@ -1048,7 +1004,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
@@ -1062,7 +1018,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -1076,7 +1032,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>4</v>
       </c>
@@ -1090,7 +1046,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>4</v>
       </c>
@@ -1104,7 +1060,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>4</v>
       </c>
@@ -1118,7 +1074,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>4</v>
       </c>
@@ -1132,7 +1088,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>4</v>
       </c>
@@ -1146,7 +1102,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>4</v>
       </c>
@@ -1160,7 +1116,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>4</v>
       </c>
@@ -1188,7 +1144,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>4</v>
       </c>
@@ -1202,7 +1158,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>4</v>
       </c>
@@ -1230,7 +1186,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>4</v>
       </c>
@@ -1244,7 +1200,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>4</v>
       </c>
@@ -1258,7 +1214,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>4</v>
       </c>
@@ -1272,7 +1228,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>4</v>
       </c>
@@ -1286,7 +1242,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>4</v>
       </c>
@@ -1300,7 +1256,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>35</v>
       </c>
@@ -1314,7 +1270,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>35</v>
       </c>
@@ -1328,7 +1284,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>35</v>
       </c>
@@ -1342,7 +1298,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>35</v>
       </c>
@@ -1356,7 +1312,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
@@ -1370,7 +1326,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
@@ -1384,7 +1340,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>35</v>
       </c>
@@ -1398,7 +1354,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>35</v>
       </c>
@@ -1412,7 +1368,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>35</v>
       </c>
@@ -1426,7 +1382,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>35</v>
       </c>
@@ -1440,7 +1396,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>35</v>
       </c>
@@ -1454,7 +1410,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>35</v>
       </c>
@@ -1468,7 +1424,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>35</v>
       </c>
@@ -1482,7 +1438,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>35</v>
       </c>
@@ -1496,7 +1452,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>35</v>
       </c>
@@ -1510,7 +1466,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>35</v>
       </c>
@@ -1524,7 +1480,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>35</v>
       </c>
@@ -1538,7 +1494,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>35</v>
       </c>
@@ -1552,7 +1508,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>35</v>
       </c>
@@ -1566,7 +1522,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>35</v>
       </c>
@@ -1594,7 +1550,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>35</v>
       </c>
@@ -1608,7 +1564,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>35</v>
       </c>
@@ -1636,7 +1592,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>35</v>
       </c>
@@ -1650,7 +1606,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>35</v>
       </c>
@@ -1664,7 +1620,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>35</v>
       </c>
@@ -1678,7 +1634,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>35</v>
       </c>
@@ -1692,7 +1648,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>35</v>
       </c>
@@ -1706,7 +1662,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>36</v>
       </c>
@@ -1720,7 +1676,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>36</v>
       </c>
@@ -1734,7 +1690,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>36</v>
       </c>
@@ -1748,7 +1704,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>36</v>
       </c>
@@ -1762,7 +1718,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>36</v>
       </c>
@@ -1776,7 +1732,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>36</v>
       </c>
@@ -1790,7 +1746,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>36</v>
       </c>
@@ -1804,7 +1760,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>36</v>
       </c>
@@ -1818,7 +1774,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>36</v>
       </c>
@@ -1832,7 +1788,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>36</v>
       </c>
@@ -1846,7 +1802,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>36</v>
       </c>
@@ -1860,7 +1816,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>36</v>
       </c>
@@ -1874,7 +1830,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>36</v>
       </c>
@@ -1888,7 +1844,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>36</v>
       </c>
@@ -1902,7 +1858,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>36</v>
       </c>
@@ -1916,7 +1872,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>36</v>
       </c>
@@ -1930,7 +1886,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="77" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>36</v>
       </c>
@@ -1944,7 +1900,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>36</v>
       </c>
@@ -1958,7 +1914,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="79" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>36</v>
       </c>
@@ -1986,7 +1942,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="81" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>36</v>
       </c>
@@ -2000,7 +1956,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>36</v>
       </c>
@@ -2028,7 +1984,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>36</v>
       </c>
@@ -2042,7 +1998,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="85" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>36</v>
       </c>
@@ -2056,7 +2012,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="86" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>36</v>
       </c>
@@ -2070,7 +2026,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="87" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>36</v>
       </c>
@@ -2084,7 +2040,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="88" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>36</v>
       </c>
@@ -2098,7 +2054,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="89" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>37</v>
       </c>
@@ -2112,7 +2068,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="90" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>37</v>
       </c>
@@ -2126,7 +2082,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="91" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>37</v>
       </c>
@@ -2140,7 +2096,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="92" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>37</v>
       </c>
@@ -2154,7 +2110,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="93" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>37</v>
       </c>
@@ -2168,7 +2124,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="94" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>37</v>
       </c>
@@ -2182,7 +2138,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="95" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>37</v>
       </c>
@@ -2196,7 +2152,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="96" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>37</v>
       </c>
@@ -2210,7 +2166,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="97" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>37</v>
       </c>
@@ -2224,7 +2180,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="98" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>37</v>
       </c>
@@ -2238,7 +2194,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="99" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>37</v>
       </c>
@@ -2252,7 +2208,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="100" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>37</v>
       </c>
@@ -2266,7 +2222,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="101" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>37</v>
       </c>
@@ -2280,7 +2236,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="102" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>37</v>
       </c>
@@ -2294,7 +2250,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="103" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>37</v>
       </c>
@@ -2308,7 +2264,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="104" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>37</v>
       </c>
@@ -2322,7 +2278,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="105" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>37</v>
       </c>
@@ -2336,7 +2292,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="106" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>37</v>
       </c>
@@ -2364,7 +2320,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="108" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>37</v>
       </c>
@@ -2378,7 +2334,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="109" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>37</v>
       </c>
@@ -2406,7 +2362,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="111" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>37</v>
       </c>
@@ -2420,7 +2376,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="112" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>37</v>
       </c>
@@ -2434,7 +2390,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="113" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>37</v>
       </c>
@@ -2448,7 +2404,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="114" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>37</v>
       </c>
@@ -2462,7 +2418,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="115" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>37</v>
       </c>
@@ -2476,7 +2432,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="116" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>38</v>
       </c>
@@ -2490,7 +2446,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="117" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>38</v>
       </c>
@@ -2504,7 +2460,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="118" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>38</v>
       </c>
@@ -2518,7 +2474,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="119" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>38</v>
       </c>
@@ -2532,7 +2488,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="120" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>38</v>
       </c>
@@ -2546,7 +2502,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="121" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>38</v>
       </c>
@@ -2560,7 +2516,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="122" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>38</v>
       </c>
@@ -2574,7 +2530,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="123" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>38</v>
       </c>
@@ -2588,7 +2544,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="124" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>38</v>
       </c>
@@ -2602,7 +2558,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="125" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>38</v>
       </c>
@@ -2616,7 +2572,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="126" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>38</v>
       </c>
@@ -2630,7 +2586,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="127" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>38</v>
       </c>
@@ -2644,7 +2600,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="128" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>38</v>
       </c>
@@ -2658,7 +2614,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="129" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
         <v>38</v>
       </c>
@@ -2672,7 +2628,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>38</v>
       </c>
@@ -2686,7 +2642,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
         <v>38</v>
       </c>
@@ -2700,7 +2656,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
         <v>38</v>
       </c>
@@ -2714,7 +2670,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
         <v>38</v>
       </c>
@@ -2728,7 +2684,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
         <v>38</v>
       </c>
@@ -2756,7 +2712,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
         <v>38</v>
       </c>
@@ -2770,7 +2726,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="137" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
         <v>38</v>
       </c>
@@ -2798,7 +2754,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="139" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
         <v>38</v>
       </c>
@@ -2812,7 +2768,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
         <v>38</v>
       </c>
@@ -2826,7 +2782,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="141" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
         <v>38</v>
       </c>
@@ -2840,7 +2796,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="142" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
         <v>38</v>
       </c>
@@ -2854,7 +2810,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="143" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
         <v>38</v>
       </c>
@@ -2868,7 +2824,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="144" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
         <v>41</v>
       </c>
@@ -2882,7 +2838,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="145" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
         <v>41</v>
       </c>
@@ -2896,7 +2852,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="146" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
         <v>41</v>
       </c>
@@ -2910,7 +2866,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="147" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
         <v>41</v>
       </c>
@@ -2924,7 +2880,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="148" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
         <v>41</v>
       </c>
@@ -2938,7 +2894,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="149" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
         <v>41</v>
       </c>
@@ -2952,7 +2908,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="150" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
         <v>41</v>
       </c>
@@ -2966,7 +2922,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="151" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
         <v>41</v>
       </c>
@@ -2980,7 +2936,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="152" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
         <v>41</v>
       </c>
@@ -2994,7 +2950,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="153" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
         <v>41</v>
       </c>
@@ -3008,7 +2964,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="154" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
         <v>41</v>
       </c>
@@ -3022,7 +2978,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="155" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
         <v>41</v>
       </c>
@@ -3036,7 +2992,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="156" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
         <v>41</v>
       </c>
@@ -3050,7 +3006,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="157" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
         <v>41</v>
       </c>
@@ -3064,7 +3020,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="158" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
         <v>41</v>
       </c>
@@ -3078,7 +3034,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="159" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
         <v>41</v>
       </c>
@@ -3106,7 +3062,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="161" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
         <v>41</v>
       </c>
@@ -3120,7 +3076,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="162" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
         <v>41</v>
       </c>
@@ -3148,7 +3104,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="164" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
         <v>41</v>
       </c>
@@ -3162,7 +3118,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="165" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" s="1" t="s">
         <v>41</v>
       </c>
@@ -3176,7 +3132,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="166" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
         <v>41</v>
       </c>
@@ -3190,7 +3146,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="167" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
         <v>41</v>
       </c>
@@ -3204,7 +3160,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="168" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
         <v>41</v>
       </c>
@@ -3218,7 +3174,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="169" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" s="1" t="s">
         <v>42</v>
       </c>
@@ -3232,7 +3188,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="170" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
         <v>42</v>
       </c>
@@ -3246,7 +3202,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="171" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" s="1" t="s">
         <v>42</v>
       </c>
@@ -3260,7 +3216,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="172" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" s="1" t="s">
         <v>42</v>
       </c>
@@ -3274,7 +3230,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="173" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" s="1" t="s">
         <v>43</v>
       </c>
@@ -3288,7 +3244,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="174" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
         <v>43</v>
       </c>
@@ -3302,7 +3258,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="175" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" s="1" t="s">
         <v>43</v>
       </c>
@@ -3316,7 +3272,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="176" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" s="1" t="s">
         <v>43</v>
       </c>
@@ -3330,7 +3286,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="177" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" s="1" t="s">
         <v>43</v>
       </c>
@@ -3344,7 +3300,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="178" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" s="1" t="s">
         <v>43</v>
       </c>
@@ -3358,7 +3314,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="179" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" s="1" t="s">
         <v>43</v>
       </c>
@@ -3372,7 +3328,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="180" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" s="1" t="s">
         <v>43</v>
       </c>
@@ -3386,7 +3342,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="181" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" s="1" t="s">
         <v>43</v>
       </c>
@@ -3400,7 +3356,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="182" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" s="1" t="s">
         <v>43</v>
       </c>
@@ -3414,7 +3370,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="183" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" s="1" t="s">
         <v>43</v>
       </c>
@@ -3428,7 +3384,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="184" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
         <v>43</v>
       </c>
@@ -3442,7 +3398,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="185" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" s="1" t="s">
         <v>43</v>
       </c>
@@ -3456,7 +3412,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="186" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">
         <v>43</v>
       </c>
@@ -3470,7 +3426,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="187" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" s="1" t="s">
         <v>43</v>
       </c>
@@ -3498,7 +3454,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="189" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" s="1" t="s">
         <v>43</v>
       </c>
@@ -3512,7 +3468,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="190" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" s="1" t="s">
         <v>43</v>
       </c>
@@ -3540,7 +3496,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="192" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" s="1" t="s">
         <v>43</v>
       </c>
@@ -3554,7 +3510,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="193" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" s="1" t="s">
         <v>43</v>
       </c>
@@ -3568,7 +3524,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="194" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" s="1" t="s">
         <v>43</v>
       </c>
@@ -3582,7 +3538,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="195" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" s="1" t="s">
         <v>43</v>
       </c>
@@ -3596,7 +3552,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="196" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" s="1" t="s">
         <v>43</v>
       </c>
@@ -3610,7 +3566,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="197" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" s="1" t="s">
         <v>44</v>
       </c>
@@ -3624,7 +3580,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="198" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" s="1" t="s">
         <v>44</v>
       </c>
@@ -3638,7 +3594,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="199" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" s="1" t="s">
         <v>44</v>
       </c>
@@ -3652,7 +3608,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="200" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" s="1" t="s">
         <v>44</v>
       </c>
@@ -3666,7 +3622,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="201" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" s="1" t="s">
         <v>44</v>
       </c>
@@ -3680,7 +3636,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="202" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" s="1" t="s">
         <v>44</v>
       </c>
@@ -3694,7 +3650,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="203" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" s="1" t="s">
         <v>44</v>
       </c>
@@ -3708,7 +3664,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="204" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" s="1" t="s">
         <v>44</v>
       </c>
@@ -3722,7 +3678,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="205" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" s="1" t="s">
         <v>44</v>
       </c>
@@ -3736,7 +3692,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="206" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" s="1" t="s">
         <v>44</v>
       </c>
@@ -3750,7 +3706,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="207" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" s="1" t="s">
         <v>44</v>
       </c>
@@ -3764,7 +3720,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="208" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" s="1" t="s">
         <v>44</v>
       </c>
@@ -3778,7 +3734,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="209" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" s="1" t="s">
         <v>44</v>
       </c>
@@ -3792,7 +3748,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="210" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" s="1" t="s">
         <v>44</v>
       </c>
@@ -3820,7 +3776,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="212" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" s="1" t="s">
         <v>44</v>
       </c>
@@ -3834,7 +3790,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="213" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" s="1" t="s">
         <v>44</v>
       </c>
@@ -3862,7 +3818,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="215" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" s="1" t="s">
         <v>44</v>
       </c>
@@ -3876,7 +3832,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="216" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216" s="1" t="s">
         <v>44</v>
       </c>
@@ -3890,7 +3846,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="217" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" s="1" t="s">
         <v>44</v>
       </c>
@@ -3904,7 +3860,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="218" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218" s="1" t="s">
         <v>44</v>
       </c>
@@ -3918,7 +3874,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="219" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" s="1" t="s">
         <v>44</v>
       </c>
@@ -3932,7 +3888,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="220" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" s="1" t="s">
         <v>45</v>
       </c>
@@ -3946,7 +3902,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="221" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" s="1" t="s">
         <v>45</v>
       </c>
@@ -3960,7 +3916,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="222" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" s="1" t="s">
         <v>45</v>
       </c>
@@ -3974,7 +3930,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="223" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" s="1" t="s">
         <v>45</v>
       </c>
@@ -3988,7 +3944,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="224" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224" s="1" t="s">
         <v>45</v>
       </c>
@@ -4002,7 +3958,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="225" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" s="1" t="s">
         <v>45</v>
       </c>
@@ -4016,7 +3972,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="226" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" s="1" t="s">
         <v>45</v>
       </c>
@@ -4030,7 +3986,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="227" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" s="1" t="s">
         <v>45</v>
       </c>
@@ -4044,7 +4000,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="228" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" s="1" t="s">
         <v>45</v>
       </c>
@@ -4058,7 +4014,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="229" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" s="1" t="s">
         <v>45</v>
       </c>
@@ -4072,7 +4028,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="230" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230" s="1" t="s">
         <v>45</v>
       </c>
@@ -4086,7 +4042,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="231" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231" s="1" t="s">
         <v>45</v>
       </c>
@@ -4100,7 +4056,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="232" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232" s="1" t="s">
         <v>45</v>
       </c>
@@ -4128,7 +4084,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="234" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A234" s="1" t="s">
         <v>45</v>
       </c>
@@ -4142,7 +4098,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="235" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A235" s="1" t="s">
         <v>45</v>
       </c>
@@ -4170,7 +4126,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="237" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A237" s="1" t="s">
         <v>45</v>
       </c>
@@ -4184,7 +4140,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="238" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A238" s="1" t="s">
         <v>45</v>
       </c>
@@ -4198,7 +4154,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="239" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A239" s="1" t="s">
         <v>45</v>
       </c>
@@ -4212,7 +4168,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="240" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A240" s="1" t="s">
         <v>45</v>
       </c>
@@ -4226,7 +4182,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="241" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A241" s="1" t="s">
         <v>45</v>
       </c>
@@ -4240,7 +4196,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="242" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A242" s="1" t="s">
         <v>46</v>
       </c>
@@ -4254,7 +4210,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="243" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A243" s="1" t="s">
         <v>46</v>
       </c>
@@ -4268,7 +4224,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="244" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A244" s="1" t="s">
         <v>46</v>
       </c>
@@ -4282,7 +4238,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="245" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A245" s="1" t="s">
         <v>46</v>
       </c>
@@ -4296,7 +4252,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="246" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A246" s="1" t="s">
         <v>46</v>
       </c>
@@ -4310,7 +4266,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="247" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A247" s="1" t="s">
         <v>46</v>
       </c>
@@ -4324,7 +4280,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="248" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A248" s="1" t="s">
         <v>46</v>
       </c>
@@ -4338,7 +4294,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="249" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A249" s="1" t="s">
         <v>46</v>
       </c>
@@ -4352,7 +4308,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="250" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A250" s="1" t="s">
         <v>46</v>
       </c>
@@ -4366,7 +4322,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="251" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A251" s="1" t="s">
         <v>46</v>
       </c>
@@ -4380,7 +4336,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="252" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A252" s="1" t="s">
         <v>46</v>
       </c>
@@ -4394,7 +4350,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="253" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A253" s="1" t="s">
         <v>46</v>
       </c>
@@ -4422,7 +4378,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="255" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A255" s="1" t="s">
         <v>46</v>
       </c>
@@ -4436,7 +4392,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="256" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A256" s="1" t="s">
         <v>46</v>
       </c>
@@ -4464,7 +4420,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="258" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A258" s="1" t="s">
         <v>46</v>
       </c>
@@ -4478,7 +4434,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="259" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A259" s="1" t="s">
         <v>46</v>
       </c>
@@ -4492,7 +4448,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="260" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A260" s="1" t="s">
         <v>46</v>
       </c>
@@ -4506,7 +4462,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="261" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A261" s="1" t="s">
         <v>46</v>
       </c>
@@ -4520,7 +4476,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="262" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A262" s="1" t="s">
         <v>46</v>
       </c>
@@ -4534,7 +4490,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="263" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A263" s="1" t="s">
         <v>47</v>
       </c>
@@ -4548,7 +4504,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="264" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A264" s="1" t="s">
         <v>47</v>
       </c>
@@ -4562,7 +4518,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="265" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A265" s="1" t="s">
         <v>47</v>
       </c>
@@ -4576,7 +4532,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="266" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A266" s="1" t="s">
         <v>48</v>
       </c>
@@ -4590,7 +4546,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="267" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A267" s="1" t="s">
         <v>48</v>
       </c>
@@ -4604,7 +4560,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="268" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A268" s="1" t="s">
         <v>48</v>
       </c>
@@ -4618,7 +4574,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="269" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A269" s="1" t="s">
         <v>48</v>
       </c>
@@ -4632,7 +4588,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="270" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A270" s="1" t="s">
         <v>48</v>
       </c>
@@ -4646,7 +4602,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="271" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A271" s="1" t="s">
         <v>48</v>
       </c>
@@ -4660,7 +4616,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="272" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A272" s="1" t="s">
         <v>48</v>
       </c>
@@ -4674,7 +4630,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="273" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A273" s="1" t="s">
         <v>48</v>
       </c>
@@ -4688,7 +4644,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="274" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A274" s="1" t="s">
         <v>48</v>
       </c>
@@ -4702,7 +4658,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="275" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A275" s="1" t="s">
         <v>48</v>
       </c>
@@ -4716,7 +4672,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="276" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A276" s="1" t="s">
         <v>48</v>
       </c>
@@ -4744,7 +4700,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="278" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A278" s="1" t="s">
         <v>48</v>
       </c>
@@ -4758,7 +4714,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="279" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A279" s="1" t="s">
         <v>48</v>
       </c>
@@ -4786,7 +4742,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="281" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A281" s="1" t="s">
         <v>48</v>
       </c>
@@ -4800,7 +4756,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="282" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A282" s="1" t="s">
         <v>48</v>
       </c>
@@ -4814,7 +4770,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="283" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A283" s="1" t="s">
         <v>48</v>
       </c>
@@ -4828,7 +4784,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="284" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A284" s="1" t="s">
         <v>48</v>
       </c>
@@ -4842,7 +4798,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="285" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A285" s="1" t="s">
         <v>48</v>
       </c>
@@ -4856,7 +4812,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="286" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A286" s="1" t="s">
         <v>49</v>
       </c>
@@ -4870,7 +4826,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="287" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A287" s="1" t="s">
         <v>49</v>
       </c>
@@ -4884,7 +4840,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="288" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A288" s="1" t="s">
         <v>49</v>
       </c>
@@ -4898,7 +4854,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="289" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A289" s="1" t="s">
         <v>49</v>
       </c>
@@ -4912,7 +4868,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="290" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A290" s="1" t="s">
         <v>49</v>
       </c>
@@ -4926,7 +4882,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="291" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A291" s="1" t="s">
         <v>49</v>
       </c>
@@ -4940,7 +4896,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="292" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A292" s="1" t="s">
         <v>49</v>
       </c>
@@ -4954,7 +4910,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="293" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A293" s="1" t="s">
         <v>49</v>
       </c>
@@ -4968,7 +4924,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="294" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A294" s="1" t="s">
         <v>49</v>
       </c>
@@ -4982,7 +4938,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="295" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A295" s="1" t="s">
         <v>49</v>
       </c>
@@ -5010,7 +4966,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="297" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A297" s="1" t="s">
         <v>49</v>
       </c>
@@ -5024,7 +4980,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="298" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A298" s="1" t="s">
         <v>49</v>
       </c>
@@ -5052,7 +5008,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="300" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A300" s="1" t="s">
         <v>49</v>
       </c>
@@ -5066,7 +5022,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="301" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A301" s="1" t="s">
         <v>49</v>
       </c>
@@ -5080,7 +5036,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="302" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A302" s="1" t="s">
         <v>49</v>
       </c>
@@ -5094,7 +5050,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="303" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A303" s="1" t="s">
         <v>49</v>
       </c>
@@ -5108,7 +5064,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="304" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A304" s="1" t="s">
         <v>49</v>
       </c>
@@ -5122,7 +5078,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="305" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A305" s="1" t="s">
         <v>50</v>
       </c>
@@ -5136,7 +5092,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="306" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A306" s="1" t="s">
         <v>50</v>
       </c>
@@ -5150,7 +5106,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="307" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A307" s="1" t="s">
         <v>50</v>
       </c>
@@ -5164,7 +5120,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="308" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A308" s="1" t="s">
         <v>50</v>
       </c>
@@ -5178,7 +5134,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="309" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A309" s="1" t="s">
         <v>50</v>
       </c>
@@ -5192,7 +5148,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="310" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A310" s="1" t="s">
         <v>50</v>
       </c>
@@ -5206,7 +5162,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="311" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A311" s="1" t="s">
         <v>50</v>
       </c>
@@ -5220,7 +5176,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="312" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A312" s="1" t="s">
         <v>50</v>
       </c>
@@ -5234,7 +5190,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="313" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A313" s="1" t="s">
         <v>50</v>
       </c>
@@ -5262,7 +5218,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="315" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A315" s="1" t="s">
         <v>50</v>
       </c>
@@ -5276,7 +5232,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="316" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A316" s="1" t="s">
         <v>50</v>
       </c>
@@ -5304,7 +5260,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="318" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A318" s="1" t="s">
         <v>50</v>
       </c>
@@ -5318,7 +5274,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="319" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A319" s="1" t="s">
         <v>50</v>
       </c>
@@ -5332,7 +5288,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="320" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A320" s="1" t="s">
         <v>50</v>
       </c>
@@ -5346,7 +5302,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="321" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A321" s="1" t="s">
         <v>50</v>
       </c>
@@ -5360,7 +5316,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="322" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A322" s="1" t="s">
         <v>50</v>
       </c>
@@ -5374,7 +5330,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="323" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A323" s="1" t="s">
         <v>51</v>
       </c>
@@ -5388,7 +5344,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="324" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A324" s="1" t="s">
         <v>51</v>
       </c>
@@ -5402,7 +5358,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="325" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A325" s="1" t="s">
         <v>51</v>
       </c>
@@ -5416,7 +5372,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="326" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A326" s="1" t="s">
         <v>51</v>
       </c>
@@ -5430,7 +5386,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="327" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A327" s="1" t="s">
         <v>51</v>
       </c>
@@ -5444,7 +5400,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="328" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A328" s="1" t="s">
         <v>51</v>
       </c>
@@ -5458,7 +5414,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="329" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A329" s="1" t="s">
         <v>51</v>
       </c>
@@ -5472,7 +5428,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="330" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A330" s="1" t="s">
         <v>51</v>
       </c>
@@ -5500,7 +5456,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="332" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A332" s="1" t="s">
         <v>51</v>
       </c>
@@ -5514,7 +5470,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="333" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A333" s="1" t="s">
         <v>51</v>
       </c>
@@ -5542,7 +5498,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="335" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A335" s="1" t="s">
         <v>51</v>
       </c>
@@ -5556,7 +5512,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="336" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A336" s="1" t="s">
         <v>51</v>
       </c>
@@ -5570,7 +5526,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="337" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A337" s="1" t="s">
         <v>51</v>
       </c>
@@ -5584,7 +5540,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="338" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A338" s="1" t="s">
         <v>51</v>
       </c>
@@ -5598,7 +5554,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="339" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A339" s="1" t="s">
         <v>51</v>
       </c>
@@ -5612,7 +5568,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="340" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A340" s="1" t="s">
         <v>52</v>
       </c>
@@ -5626,7 +5582,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="341" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A341" s="1" t="s">
         <v>52</v>
       </c>
@@ -5640,7 +5596,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="342" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A342" s="1" t="s">
         <v>52</v>
       </c>
@@ -5654,7 +5610,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="343" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A343" s="1" t="s">
         <v>52</v>
       </c>
@@ -5668,7 +5624,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="344" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A344" s="1" t="s">
         <v>52</v>
       </c>
@@ -5682,7 +5638,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="345" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A345" s="1" t="s">
         <v>52</v>
       </c>
@@ -5696,7 +5652,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="346" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A346" s="1" t="s">
         <v>52</v>
       </c>
@@ -5724,7 +5680,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="348" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A348" s="1" t="s">
         <v>52</v>
       </c>
@@ -5738,7 +5694,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="349" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A349" s="1" t="s">
         <v>52</v>
       </c>
@@ -5766,7 +5722,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="351" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A351" s="1" t="s">
         <v>52</v>
       </c>
@@ -5780,7 +5736,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="352" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A352" s="1" t="s">
         <v>52</v>
       </c>
@@ -5794,7 +5750,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="353" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A353" s="1" t="s">
         <v>52</v>
       </c>
@@ -5808,7 +5764,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="354" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A354" s="1" t="s">
         <v>52</v>
       </c>
@@ -5822,7 +5778,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="355" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A355" s="1" t="s">
         <v>52</v>
       </c>
@@ -5836,7 +5792,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="356" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A356" s="1" t="s">
         <v>53</v>
       </c>
@@ -5850,7 +5806,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="357" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A357" s="1" t="s">
         <v>53</v>
       </c>
@@ -5864,7 +5820,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="358" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A358" s="1" t="s">
         <v>53</v>
       </c>
@@ -5878,7 +5834,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="359" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A359" s="1" t="s">
         <v>53</v>
       </c>
@@ -5892,7 +5848,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="360" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A360" s="1" t="s">
         <v>53</v>
       </c>
@@ -5906,7 +5862,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="361" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A361" s="1" t="s">
         <v>53</v>
       </c>
@@ -5934,7 +5890,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="363" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A363" s="1" t="s">
         <v>53</v>
       </c>
@@ -5948,7 +5904,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="364" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A364" s="1" t="s">
         <v>53</v>
       </c>
@@ -5976,7 +5932,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="366" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A366" s="1" t="s">
         <v>53</v>
       </c>
@@ -5990,7 +5946,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="367" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A367" s="1" t="s">
         <v>53</v>
       </c>
@@ -6004,7 +5960,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="368" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A368" s="1" t="s">
         <v>53</v>
       </c>
@@ -6018,7 +5974,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="369" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A369" s="1" t="s">
         <v>53</v>
       </c>
@@ -6032,7 +5988,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="370" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A370" s="1" t="s">
         <v>53</v>
       </c>
@@ -6046,7 +6002,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="371" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A371" s="1" t="s">
         <v>54</v>
       </c>
@@ -6060,7 +6016,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="372" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A372" s="1" t="s">
         <v>54</v>
       </c>
@@ -6074,7 +6030,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="373" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A373" s="1" t="s">
         <v>54</v>
       </c>
@@ -6088,7 +6044,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="374" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A374" s="1" t="s">
         <v>54</v>
       </c>
@@ -6102,7 +6058,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="375" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A375" s="1" t="s">
         <v>54</v>
       </c>
@@ -6130,7 +6086,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="377" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A377" s="1" t="s">
         <v>54</v>
       </c>
@@ -6144,7 +6100,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="378" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A378" s="1" t="s">
         <v>54</v>
       </c>
@@ -6172,7 +6128,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="380" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A380" s="1" t="s">
         <v>54</v>
       </c>
@@ -6186,7 +6142,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="381" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A381" s="1" t="s">
         <v>54</v>
       </c>
@@ -6200,7 +6156,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="382" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A382" s="1" t="s">
         <v>54</v>
       </c>
@@ -6214,7 +6170,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="383" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A383" s="1" t="s">
         <v>54</v>
       </c>
@@ -6228,7 +6184,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="384" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A384" s="1" t="s">
         <v>54</v>
       </c>
@@ -6242,7 +6198,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="385" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A385" s="1" t="s">
         <v>55</v>
       </c>
@@ -6256,7 +6212,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="386" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A386" s="1" t="s">
         <v>55</v>
       </c>
@@ -6270,7 +6226,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="387" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A387" s="1" t="s">
         <v>55</v>
       </c>
@@ -6284,7 +6240,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="388" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A388" s="1" t="s">
         <v>55</v>
       </c>
@@ -6312,7 +6268,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="390" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A390" s="1" t="s">
         <v>55</v>
       </c>
@@ -6326,7 +6282,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="391" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A391" s="1" t="s">
         <v>55</v>
       </c>
@@ -6354,7 +6310,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="393" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A393" s="1" t="s">
         <v>55</v>
       </c>
@@ -6368,7 +6324,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="394" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A394" s="1" t="s">
         <v>55</v>
       </c>
@@ -6382,7 +6338,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="395" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A395" s="1" t="s">
         <v>55</v>
       </c>
@@ -6396,7 +6352,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="396" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A396" s="1" t="s">
         <v>55</v>
       </c>
@@ -6410,7 +6366,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="397" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A397" s="1" t="s">
         <v>55</v>
       </c>
@@ -6424,7 +6380,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="398" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A398" s="1" t="s">
         <v>56</v>
       </c>
@@ -6438,7 +6394,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="399" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A399" s="1" t="s">
         <v>56</v>
       </c>
@@ -6452,7 +6408,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="400" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A400" s="1" t="s">
         <v>56</v>
       </c>
@@ -6480,7 +6436,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="402" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A402" s="1" t="s">
         <v>56</v>
       </c>
@@ -6494,7 +6450,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="403" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A403" s="1" t="s">
         <v>56</v>
       </c>
@@ -6522,7 +6478,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="405" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A405" s="1" t="s">
         <v>56</v>
       </c>
@@ -6536,7 +6492,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="406" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A406" s="1" t="s">
         <v>56</v>
       </c>
@@ -6550,7 +6506,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="407" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A407" s="1" t="s">
         <v>56</v>
       </c>
@@ -6564,7 +6520,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="408" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A408" s="1" t="s">
         <v>56</v>
       </c>
@@ -6578,7 +6534,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="409" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A409" s="1" t="s">
         <v>56</v>
       </c>
@@ -6592,7 +6548,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="410" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A410" s="1" t="s">
         <v>57</v>
       </c>
@@ -6606,7 +6562,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="411" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A411" s="1" t="s">
         <v>57</v>
       </c>
@@ -6634,7 +6590,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="413" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A413" s="1" t="s">
         <v>57</v>
       </c>
@@ -6648,7 +6604,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="414" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A414" s="1" t="s">
         <v>57</v>
       </c>
@@ -6676,7 +6632,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="416" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A416" s="1" t="s">
         <v>57</v>
       </c>
@@ -6690,7 +6646,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="417" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A417" s="1" t="s">
         <v>57</v>
       </c>
@@ -6704,7 +6660,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="418" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A418" s="1" t="s">
         <v>57</v>
       </c>
@@ -6718,7 +6674,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="419" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A419" s="1" t="s">
         <v>57</v>
       </c>
@@ -6732,7 +6688,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="420" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A420" s="1" t="s">
         <v>57</v>
       </c>
@@ -6746,7 +6702,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="421" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A421" s="1" t="s">
         <v>58</v>
       </c>
@@ -6774,7 +6730,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="423" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A423" s="1" t="s">
         <v>58</v>
       </c>
@@ -6788,7 +6744,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="424" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A424" s="1" t="s">
         <v>58</v>
       </c>
@@ -6816,7 +6772,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="426" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A426" s="1" t="s">
         <v>58</v>
       </c>
@@ -6830,7 +6786,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="427" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A427" s="1" t="s">
         <v>58</v>
       </c>
@@ -6844,7 +6800,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="428" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A428" s="1" t="s">
         <v>58</v>
       </c>
@@ -6858,7 +6814,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="429" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A429" s="1" t="s">
         <v>58</v>
       </c>
@@ -6872,7 +6828,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="430" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A430" s="1" t="s">
         <v>58</v>
       </c>
@@ -6900,7 +6856,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="432" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A432" s="1" t="s">
         <v>59</v>
       </c>
@@ -6914,7 +6870,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="433" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A433" s="1" t="s">
         <v>59</v>
       </c>
@@ -6942,7 +6898,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="435" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A435" s="1" t="s">
         <v>59</v>
       </c>
@@ -6956,7 +6912,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="436" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A436" s="1" t="s">
         <v>59</v>
       </c>
@@ -6970,7 +6926,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="437" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A437" s="1" t="s">
         <v>59</v>
       </c>
@@ -6984,7 +6940,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="438" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A438" s="1" t="s">
         <v>59</v>
       </c>
@@ -6998,7 +6954,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="439" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A439" s="1" t="s">
         <v>59</v>
       </c>
@@ -7012,7 +6968,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="440" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A440" s="1" t="s">
         <v>60</v>
       </c>
@@ -7026,7 +6982,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="441" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A441" s="1" t="s">
         <v>60</v>
       </c>
@@ -7040,7 +6996,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="442" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A442" s="1" t="s">
         <v>60</v>
       </c>
@@ -7054,7 +7010,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="443" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="443" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A443" s="1" t="s">
         <v>60</v>
       </c>
@@ -7068,7 +7024,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="444" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A444" s="1" t="s">
         <v>60</v>
       </c>
@@ -7082,7 +7038,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="445" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="445" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A445" s="1" t="s">
         <v>60</v>
       </c>
@@ -7096,7 +7052,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="446" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A446" s="1" t="s">
         <v>60</v>
       </c>
@@ -7110,7 +7066,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="447" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A447" s="1" t="s">
         <v>60</v>
       </c>
@@ -7124,7 +7080,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="448" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="448" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A448" s="1" t="s">
         <v>61</v>
       </c>
@@ -7152,7 +7108,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="450" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="450" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A450" s="1" t="s">
         <v>61</v>
       </c>
@@ -7166,7 +7122,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="451" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="451" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A451" s="1" t="s">
         <v>61</v>
       </c>
@@ -7180,7 +7136,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="452" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="452" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A452" s="1" t="s">
         <v>61</v>
       </c>
@@ -7194,7 +7150,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="453" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="453" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A453" s="1" t="s">
         <v>61</v>
       </c>
@@ -7208,7 +7164,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="454" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="454" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A454" s="1" t="s">
         <v>61</v>
       </c>
@@ -7236,7 +7192,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="456" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="456" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A456" s="1" t="s">
         <v>62</v>
       </c>
@@ -7250,7 +7206,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="457" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="457" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A457" s="1" t="s">
         <v>62</v>
       </c>
@@ -7264,7 +7220,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="458" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="458" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A458" s="1" t="s">
         <v>62</v>
       </c>
@@ -7278,7 +7234,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="459" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="459" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A459" s="1" t="s">
         <v>62</v>
       </c>
@@ -7292,7 +7248,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="460" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="460" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A460" s="1" t="s">
         <v>62</v>
       </c>
@@ -7306,7 +7262,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="461" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="461" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A461" s="1" t="s">
         <v>63</v>
       </c>
@@ -7320,7 +7276,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="462" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="462" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A462" s="1" t="s">
         <v>63</v>
       </c>
@@ -7334,7 +7290,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="463" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="463" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A463" s="1" t="s">
         <v>63</v>
       </c>
@@ -7348,7 +7304,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="464" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="464" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A464" s="1" t="s">
         <v>67</v>
       </c>
@@ -7362,7 +7318,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="465" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="465" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A465" s="1" t="s">
         <v>67</v>
       </c>
@@ -7376,7 +7332,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="466" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="466" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A466" s="1" t="s">
         <v>67</v>
       </c>
@@ -7390,7 +7346,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="467" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="467" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A467" s="1" t="s">
         <v>67</v>
       </c>
@@ -7404,7 +7360,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="468" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="468" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A468" s="1" t="s">
         <v>67</v>
       </c>
@@ -7418,7 +7374,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="469" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="469" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A469" s="1" t="s">
         <v>68</v>
       </c>
@@ -7432,7 +7388,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="470" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="470" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A470" s="1" t="s">
         <v>68</v>
       </c>
@@ -7446,7 +7402,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="471" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="471" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A471" s="1" t="s">
         <v>68</v>
       </c>
@@ -7460,7 +7416,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="472" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="472" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A472" s="1" t="s">
         <v>68</v>
       </c>
@@ -7474,7 +7430,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="473" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="473" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A473" s="1" t="s">
         <v>69</v>
       </c>
@@ -7488,7 +7444,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="474" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="474" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A474" s="1" t="s">
         <v>69</v>
       </c>
@@ -7502,7 +7458,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="475" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="475" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A475" s="1" t="s">
         <v>69</v>
       </c>
@@ -7516,7 +7472,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="476" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="476" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A476" s="1" t="s">
         <v>70</v>
       </c>
@@ -7530,7 +7486,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="477" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="477" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A477" s="1" t="s">
         <v>70</v>
       </c>
@@ -7544,7 +7500,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="478" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="478" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A478" s="1" t="s">
         <v>71</v>
       </c>
@@ -7558,7 +7514,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="479" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="479" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A479" s="1" t="s">
         <v>71</v>
       </c>
@@ -7572,7 +7528,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="480" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="480" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A480" s="1" t="s">
         <v>72</v>
       </c>
@@ -7586,7 +7542,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="481" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="481" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A481" s="1" t="s">
         <v>73</v>
       </c>
@@ -7612,8 +7568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E78993AB-95F8-44AB-A097-D09A1AD7B453}">
   <dimension ref="A1:D341"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A306" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B341"/>
+    <sheetView topLeftCell="A306" workbookViewId="0">
+      <selection activeCell="C318" sqref="C318"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>